<commit_message>
Extract CourseData From SS file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSource/SS.xlsx
+++ b/src/main/resources/dataSource/SS.xlsx
@@ -2330,6 +2330,18 @@
   </si>
   <si>
     <t>AMARI</t>
+  </si>
+  <si>
+    <t>Mle1</t>
+  </si>
+  <si>
+    <t>Mle3</t>
+  </si>
+  <si>
+    <t>Mle2</t>
+  </si>
+  <si>
+    <t>Mle4</t>
   </si>
 </sst>
 </file>
@@ -2703,7 +2715,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2728,7 +2740,7 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>772</v>
       </c>
       <c r="H1" t="s">
         <v>11</v>
@@ -2740,7 +2752,7 @@
         <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>774</v>
       </c>
       <c r="L1" t="s">
         <v>14</v>
@@ -2752,7 +2764,7 @@
         <v>16</v>
       </c>
       <c r="O1" t="s">
-        <v>10</v>
+        <v>773</v>
       </c>
       <c r="P1" t="s">
         <v>17</v>
@@ -2764,7 +2776,7 @@
         <v>19</v>
       </c>
       <c r="S1" t="s">
-        <v>10</v>
+        <v>775</v>
       </c>
       <c r="T1" t="s">
         <v>20</v>

</xml_diff>